<commit_message>
more information in Tom Tat Luan Van
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>TomTatLuanVan</t>
+  </si>
+  <si>
+    <t>ALMOST THERE. FINISH LATER</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C1:GioiThieu - architecture done. missing algorithm
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>ALMOST THERE. FINISH LATER</t>
+  </si>
+  <si>
+    <t>MoDau</t>
+  </si>
+  <si>
+    <t>C1-GioiThieu</t>
+  </si>
+  <si>
+    <t>ARCHITECTURE DONE. MISSING ALGORITHM</t>
   </si>
 </sst>
 </file>
@@ -387,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +407,7 @@
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="3" max="3" width="43.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -452,6 +461,34 @@
       </c>
       <c r="D4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C4 Finish pathloss, half PSO
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -78,7 +78,7 @@
     <t>C4-Algorithm</t>
   </si>
   <si>
-    <t>FINISH KALMAN</t>
+    <t>FINISH PATHLOSS, HALF PSO</t>
   </si>
 </sst>
 </file>
@@ -569,6 +569,9 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
@@ -583,7 +586,7 @@
       <c r="B10" s="2"/>
       <c r="C10">
         <f>SUM(C2:C9)</f>
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish c4. init c5
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -78,7 +78,7 @@
     <t>C4-Algorithm</t>
   </si>
   <si>
-    <t>FINISH PATHLOSS, HALF PSO</t>
+    <t>C5-ImproveRSSI</t>
   </si>
 </sst>
 </file>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,28 +570,42 @@
         <v>19</v>
       </c>
       <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10">
-        <f>SUM(C2:C9)</f>
-        <v>39</v>
+      <c r="B11" s="2"/>
+      <c r="C11">
+        <f>SUM(C2:C10)</f>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
C5 - Finish introduction of antenna
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>C5-ImproveRSSI</t>
+  </si>
+  <si>
+    <t>FINISH INTRODUCTION</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,11 +589,14 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -600,7 +606,7 @@
       <c r="B11" s="2"/>
       <c r="C11">
         <f>SUM(C2:C10)</f>
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C5 Finish. Checking later
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>C5-ImproveRSSI</t>
-  </si>
-  <si>
-    <t>UPDATE FORMULA</t>
   </si>
 </sst>
 </file>
@@ -429,7 +426,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,13 +587,13 @@
         <v>20</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,7 +603,7 @@
       <c r="B11" s="2"/>
       <c r="C11">
         <f>SUM(C2:C10)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C7 Finish. C6 update diagram
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>C7-Result</t>
-  </si>
-  <si>
-    <t>INIT</t>
   </si>
 </sst>
 </file>
@@ -435,7 +432,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,13 +636,13 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -655,7 +652,7 @@
       <c r="B13" s="2"/>
       <c r="C13">
         <f>SUM(C2:C12)</f>
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add LoiCamOn and BIA
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -432,7 +432,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -483,13 +483,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
       <c r="B13" s="2"/>
       <c r="C13">
         <f>SUM(C2:C12)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>